<commit_message>
Added files to supabase DB
</commit_message>
<xml_diff>
--- a/Companies_List.xlsx
+++ b/Companies_List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,7 +19,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7659" uniqueCount="7659">
   <si>
-    <t xml:space="preserve">Company List</t>
+    <t xml:space="preserve">Company name</t>
   </si>
   <si>
     <t xml:space="preserve">Listed Symbol</t>

</xml_diff>